<commit_message>
runs xfoil and outputs results
</commit_message>
<xml_diff>
--- a/Test_Cases/Airfoil_Xfoil/arrays.xlsx
+++ b/Test_Cases/Airfoil_Xfoil/arrays.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Altitude 0m" sheetId="1" r:id="rId1"/>
-    <sheet name="Altitude 2000m" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Cl</t>
   </si>
@@ -358,277 +357,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.21</v>
-      </c>
-      <c r="C2">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>0.21</v>
-      </c>
-      <c r="G2">
-        <v>0.25</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E2">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="J2">
-        <v>0.21</v>
-      </c>
-      <c r="K2">
-        <v>0.25</v>
+      <c r="H2">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
+        <v>0.161</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
+        <v>0.008569999999999999</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>0.21</v>
-      </c>
-      <c r="C2">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>0.21</v>
-      </c>
-      <c r="G2">
-        <v>0.25</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>0.21</v>
-      </c>
-      <c r="K2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
+      <c r="H3">
+        <v>-0.0375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>